<commit_message>
Template for report done (LOO, parallel computing, diagnostic)
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riccardo.bonazzi\OneDrive - HESSO\GitHub\Articles\ITV_Covid_test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hessoit-my.sharepoint.com/personal/riccardo_bonazzi_hes-so_ch/Documents/GitHub/Articles/ITV_Covid_test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA1E276-CC75-47E1-9D6F-17D0B962C28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{0EA1E276-CC75-47E1-9D6F-17D0B962C28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DD13028-7C78-40CF-943E-DF71CDA4F47D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2681" uniqueCount="320">
   <si>
     <t>ID</t>
   </si>
@@ -1117,13 +1117,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1200,10 +1200,10 @@
   <autoFilter ref="A1:AY29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="51">
     <tableColumn id="1" xr3:uid="{6B1CEAE8-CEA1-4A4A-AE1B-E1384B94ADDE}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{4E0E1624-C8DB-4C0A-B9B2-C6241E7874CA}" name="Heure de début" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{58407823-9003-436A-AA56-AB9C72439537}" name="Heure de fin" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{4E0E1624-C8DB-4C0A-B9B2-C6241E7874CA}" name="Heure de début" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{58407823-9003-436A-AA56-AB9C72439537}" name="Heure de fin" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{2FC5D8C0-FAD9-4229-A760-9B49C482B5C7}" name="Adresse de messagerie"/>
-    <tableColumn id="5" xr3:uid="{E0918B93-D1EA-47F9-B14C-637384AA12F0}" name="Round" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E0918B93-D1EA-47F9-B14C-637384AA12F0}" name="Round" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{AF395B37-C829-4B3C-ADCC-F14E79FA04F9}" name="Langue"/>
     <tableColumn id="7" xr3:uid="{F9BE4F1A-8086-4A29-8671-2D4F6D8ACDDD}" name="Connaissez-vous quelqu'un qui a déjà fait un test COVID ?"/>
     <tableColumn id="8" xr3:uid="{9243DC8A-6CE9-4FFC-85DB-DA1FC68E4C0B}" name="Pensez-vous que les tests COVID en général sont douloureux ?"/>
@@ -6677,10 +6677,10 @@
   <dimension ref="A1:AY37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AW1" sqref="AW1:AY1"/>
+      <selection pane="bottomRight" activeCell="AP30" sqref="AP30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7667,15 +7667,11 @@
       <c r="AM7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AN7" s="2">
-        <v>0</v>
-      </c>
+      <c r="AN7" s="2"/>
       <c r="AO7" s="2">
         <v>15</v>
       </c>
-      <c r="AP7" s="2">
-        <v>0</v>
-      </c>
+      <c r="AP7" s="2"/>
       <c r="AQ7" s="2" t="s">
         <v>102</v>
       </c>
@@ -8661,15 +8657,9 @@
       <c r="AM14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AN14" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="2">
-        <v>0</v>
-      </c>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
       <c r="AQ14" s="2" t="s">
         <v>135</v>
       </c>
@@ -9529,9 +9519,7 @@
       <c r="AO20" s="2">
         <v>30</v>
       </c>
-      <c r="AP20" s="2">
-        <v>0</v>
-      </c>
+      <c r="AP20" s="2"/>
       <c r="AQ20" s="2" t="s">
         <v>84</v>
       </c>
@@ -10243,12 +10231,8 @@
       <c r="AM25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AN25" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AO25" s="2" t="s">
-        <v>233</v>
-      </c>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
       <c r="AP25" s="2">
         <v>4</v>
       </c>
@@ -10657,12 +10641,8 @@
       <c r="AM28" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AN28" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AO28" s="2">
-        <v>0</v>
-      </c>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
       <c r="AP28" s="2">
         <v>5</v>
       </c>
@@ -10783,12 +10763,8 @@
       <c r="AM29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AN29" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO29" s="2">
-        <v>0</v>
-      </c>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
       <c r="AP29" s="2">
         <v>2</v>
       </c>

</xml_diff>